<commit_message>
PIM-9640: fix asset and record imports with numeric cells (#10252)
* PIM-9640: fix asset import with numeric cells in xlsx

* PIM-9640: fix record import with numeric cells in xlsx

* PIM-9640: add changelog

* PIM-9640: clean uses
</commit_message>
<xml_diff>
--- a/src/Akeneo/AssetManager/tests/back/Common/Resources/import_valid_assets.xlsx
+++ b/src/Akeneo/AssetManager/tests/back/Common/Resources/import_valid_assets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">assetFamilyIdentifier</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">blue,green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test with numeric values</t>
   </si>
 </sst>
 </file>
@@ -98,11 +101,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,6 +122,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,8 +172,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,7 +194,202 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{C0000000-0000-0000-5000-000000000000}"/>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{A5B7EBF1-C008-4738-AFAF-F674FE77045D}">
+  <header guid="{90FBD5BF-B1FB-4C59-A65F-4CDC85845594}" dateTime="2021-01-20T15:23:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="8" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A5B7EBF1-C008-4738-AFAF-F674FE77045D}" dateTime="2021-01-20T15:24:00.000000000Z" userName=" " r:id="rId2" minRId="9" maxRId="11" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" ua="false" sId="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">designer</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" ua="false" sId="1">
+    <nc r="B4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="3" ua="false" sId="1">
+    <nc r="C4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="4" ua="false" sId="1">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Magasin Ikea</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="5" ua="false" sId="1">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ikea</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" ua="false" sId="1">
+    <nc r="G4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">blue</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" ua="false" sId="1">
+    <nc r="H4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="8" ua="false" sId="1">
+    <nc r="I4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">blue,green</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="9" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ikea</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with integer</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="10" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with integer</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numerci values</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numerci values</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numeric values</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -192,10 +401,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,13 +502,40 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PIM-9815 Reference Entity Import XLSX fails if importing Numbers into string field (#10694)
* PIM-9640: fix asset and record imports with numeric cells (#10252)

* PIM-9640: fix asset import with numeric cells in xlsx

* PIM-9640: fix record import with numeric cells in xlsx

* PIM-9640: add changelog

* PIM-9640: clean uses

* correct fix to CHANGELOG-5.0.md

* Remove CHANGELOG.md introduced by cherrypick

Co-authored-by: Nicolas Marniesse <nicolas.marniesse@akeneo.com>
Co-authored-by: rfauglas <ronan.fauglas@akeneo.com>
</commit_message>
<xml_diff>
--- a/src/Akeneo/AssetManager/tests/back/Common/Resources/import_valid_assets.xlsx
+++ b/src/Akeneo/AssetManager/tests/back/Common/Resources/import_valid_assets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">assetFamilyIdentifier</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">blue,green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test with numeric values</t>
   </si>
 </sst>
 </file>
@@ -98,11 +101,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,6 +122,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,8 +172,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,7 +194,202 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{C0000000-0000-0000-5000-000000000000}"/>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{A5B7EBF1-C008-4738-AFAF-F674FE77045D}">
+  <header guid="{90FBD5BF-B1FB-4C59-A65F-4CDC85845594}" dateTime="2021-01-20T15:23:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="8" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A5B7EBF1-C008-4738-AFAF-F674FE77045D}" dateTime="2021-01-20T15:24:00.000000000Z" userName=" " r:id="rId2" minRId="9" maxRId="11" maxSheetId="2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" ua="false" sId="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">designer</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" ua="false" sId="1">
+    <nc r="B4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="3" ua="false" sId="1">
+    <nc r="C4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="4" ua="false" sId="1">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Magasin Ikea</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="5" ua="false" sId="1">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ikea</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" ua="false" sId="1">
+    <nc r="G4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">blue</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" ua="false" sId="1">
+    <nc r="H4" t="n">
+      <v>12345</v>
+    </nc>
+  </rcc>
+  <rcc rId="8" ua="false" sId="1">
+    <nc r="I4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">blue,green</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="9" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Ikea</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with integer</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="10" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with integer</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numerci values</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" ua="false" sId="1">
+    <oc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numerci values</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E4" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Test with numeric values</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -192,10 +401,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,13 +502,40 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>